<commit_message>
Restructured dirs and added logical design doc
</commit_message>
<xml_diff>
--- a/Documentation/003-LogicalDesign/Relational_Model_Mapping.xlsx
+++ b/Documentation/003-LogicalDesign/Relational_Model_Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\LogicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\003-LogicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD697AD-EFB1-4B98-A510-7C2DED381512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C20D1D-D817-49A7-BD3E-96585347BB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{B7C97A22-F115-4181-8B0D-AEB61CB2F847}"/>
   </bookViews>
@@ -7944,8 +7944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C38153-C6DE-43F5-9F7A-64CFB0272C41}">
   <dimension ref="B1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8046,13 +8046,13 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="6" t="s">

</xml_diff>

<commit_message>
Receive and forward shipment API half done
</commit_message>
<xml_diff>
--- a/Documentation/003-LogicalDesign/Relational_Model_Mapping.xlsx
+++ b/Documentation/003-LogicalDesign/Relational_Model_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\bits\dda-assignment\courier-mgmt-group-bm\Documentation\003-LogicalDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A708810-AC96-4D89-AFCF-2E798CEE4207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A32C41-8812-4FDE-A1B5-466337A39C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{B7C97A22-F115-4181-8B0D-AEB61CB2F847}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="53">
   <si>
     <t>shipment</t>
   </si>
@@ -11109,8 +11109,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>306552</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
@@ -11118,7 +11118,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>861060</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -11133,8 +11133,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9829800" y="4411980"/>
-          <a:ext cx="7505700" cy="7620"/>
+          <a:off x="10203793" y="4437205"/>
+          <a:ext cx="6291405" cy="3416"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -11665,14 +11665,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312858</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312858</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
@@ -11689,8 +11689,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9837420" y="4213860"/>
-          <a:ext cx="0" cy="205740"/>
+          <a:off x="10210099" y="4238034"/>
+          <a:ext cx="0" cy="206791"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -12048,6 +12048,259 @@
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455448</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>8758</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455448</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>148896</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Straight Connector 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10DCE3FD-E99B-4BB3-9236-18DCB2298659}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8373241" y="4239172"/>
+          <a:ext cx="0" cy="324069"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>464207</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>586828</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Straight Connector 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A957BB40-9D46-43E3-B15E-9D47128BC8D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="4572000"/>
+          <a:ext cx="7838966" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353145</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>170005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>385380</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>96345</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Straight Arrow Connector 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2BF8BD-E153-4C62-A18B-8AE74F208B56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="966248" y="1089660"/>
+          <a:ext cx="32235" cy="478133"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>394138</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>70069</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>560552</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Straight Connector 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{956B4C38-F485-43FF-BC8F-0698429E0F9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1007241" y="1541517"/>
+          <a:ext cx="15187449" cy="35035"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>551793</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>61311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>586828</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>140138</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="Straight Connector 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A32C554-53F8-41EF-9C3D-68DFAE2CF786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="16185931" y="1532759"/>
+          <a:ext cx="35035" cy="3021724"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -12956,7 +13209,7 @@
   <dimension ref="B1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12969,13 +13222,13 @@
     <col min="6" max="6" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.88671875" style="3" bestFit="1" customWidth="1"/>
@@ -13114,7 +13367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
@@ -13141,16 +13394,16 @@
       </c>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="E18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
@@ -13173,12 +13426,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>1</v>
       </c>
@@ -13201,33 +13454,36 @@
         <v>6</v>
       </c>
       <c r="I23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="K23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="M23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="N23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="O23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="6" t="s">
+      <c r="P23" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>49</v>
       </c>

</xml_diff>